<commit_message>
This is my second commit for Screenshot and Wait
</commit_message>
<xml_diff>
--- a/Resources/Testdata/customer.xlsx
+++ b/Resources/Testdata/customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Framework2024\Actitime\Resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD516FC1-8275-41DC-B518-EFE90A92AD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AADA0E-EB71-4A36-912A-ECF9973338FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,94 +33,94 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Google1</t>
-  </si>
-  <si>
-    <t>Productbased1</t>
-  </si>
-  <si>
-    <t>Google2</t>
-  </si>
-  <si>
-    <t>Google3</t>
-  </si>
-  <si>
-    <t>Google4</t>
-  </si>
-  <si>
-    <t>Google5</t>
-  </si>
-  <si>
-    <t>Google6</t>
-  </si>
-  <si>
-    <t>Google7</t>
-  </si>
-  <si>
-    <t>Google8</t>
-  </si>
-  <si>
-    <t>Google9</t>
-  </si>
-  <si>
-    <t>Google10</t>
-  </si>
-  <si>
-    <t>Google11</t>
-  </si>
-  <si>
-    <t>Google12</t>
-  </si>
-  <si>
-    <t>Google13</t>
-  </si>
-  <si>
-    <t>Google14</t>
-  </si>
-  <si>
-    <t>Google15</t>
-  </si>
-  <si>
-    <t>Productbased2</t>
-  </si>
-  <si>
-    <t>Productbased3</t>
-  </si>
-  <si>
-    <t>Productbased4</t>
-  </si>
-  <si>
-    <t>Productbased5</t>
-  </si>
-  <si>
-    <t>Productbased6</t>
-  </si>
-  <si>
-    <t>Productbased7</t>
-  </si>
-  <si>
-    <t>Productbased8</t>
-  </si>
-  <si>
-    <t>Productbased9</t>
-  </si>
-  <si>
-    <t>Productbased10</t>
-  </si>
-  <si>
-    <t>Productbased11</t>
-  </si>
-  <si>
-    <t>Productbased12</t>
-  </si>
-  <si>
-    <t>Productbased13</t>
-  </si>
-  <si>
-    <t>Productbased14</t>
-  </si>
-  <si>
-    <t>Productbased15</t>
+    <t>Intel1</t>
+  </si>
+  <si>
+    <t>Intel2</t>
+  </si>
+  <si>
+    <t>Intel3</t>
+  </si>
+  <si>
+    <t>Intel4</t>
+  </si>
+  <si>
+    <t>Intel5</t>
+  </si>
+  <si>
+    <t>Intel6</t>
+  </si>
+  <si>
+    <t>Intel7</t>
+  </si>
+  <si>
+    <t>Intel8</t>
+  </si>
+  <si>
+    <t>Intel9</t>
+  </si>
+  <si>
+    <t>Intel10</t>
+  </si>
+  <si>
+    <t>Intel11</t>
+  </si>
+  <si>
+    <t>Intel12</t>
+  </si>
+  <si>
+    <t>Intel13</t>
+  </si>
+  <si>
+    <t>Intel14</t>
+  </si>
+  <si>
+    <t>Intel15</t>
+  </si>
+  <si>
+    <t>Servicebased15</t>
+  </si>
+  <si>
+    <t>Servicebased1</t>
+  </si>
+  <si>
+    <t>Servicebased2</t>
+  </si>
+  <si>
+    <t>Servicebased3</t>
+  </si>
+  <si>
+    <t>Servicebased4</t>
+  </si>
+  <si>
+    <t>Servicebased5</t>
+  </si>
+  <si>
+    <t>Servicebased6</t>
+  </si>
+  <si>
+    <t>Servicebased7</t>
+  </si>
+  <si>
+    <t>Servicebased8</t>
+  </si>
+  <si>
+    <t>Servicebased9</t>
+  </si>
+  <si>
+    <t>Servicebased10</t>
+  </si>
+  <si>
+    <t>Servicebased11</t>
+  </si>
+  <si>
+    <t>Servicebased12</t>
+  </si>
+  <si>
+    <t>Servicebased13</t>
+  </si>
+  <si>
+    <t>Servicebased14</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,119 +500,119 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>